<commit_message>
Добавил prefetch_related в CourseView
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Адрес страницы</t>
   </si>
@@ -39,9 +39,6 @@
   <si>
     <t xml:space="preserve">prefetch_related</t>
   </si>
-  <si>
-    <t xml:space="preserve">courses/&lt;int:id&gt;/update/</t>
-  </si>
 </sst>
 </file>
 
@@ -55,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,18 +134,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -178,20 +176,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>